<commit_message>
Alterado o max column da caregories para min
</commit_message>
<xml_diff>
--- a/data/barchart.xlsx
+++ b/data/barchart.xlsx
@@ -174,7 +174,7 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Relatorio'!$A$2:$H$5</f>
+              <f>'Relatorio'!$A$2:$A$5</f>
             </numRef>
           </cat>
           <val>
@@ -198,7 +198,7 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Relatorio'!$A$2:$H$5</f>
+              <f>'Relatorio'!$A$2:$A$5</f>
             </numRef>
           </cat>
           <val>
@@ -222,7 +222,7 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Relatorio'!$A$2:$H$5</f>
+              <f>'Relatorio'!$A$2:$A$5</f>
             </numRef>
           </cat>
           <val>
@@ -246,7 +246,7 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Relatorio'!$A$2:$H$5</f>
+              <f>'Relatorio'!$A$2:$A$5</f>
             </numRef>
           </cat>
           <val>
@@ -270,7 +270,7 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Relatorio'!$A$2:$H$5</f>
+              <f>'Relatorio'!$A$2:$A$5</f>
             </numRef>
           </cat>
           <val>
@@ -294,7 +294,7 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Relatorio'!$A$2:$H$5</f>
+              <f>'Relatorio'!$A$2:$A$5</f>
             </numRef>
           </cat>
           <val>
@@ -318,7 +318,7 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Relatorio'!$A$2:$H$5</f>
+              <f>'Relatorio'!$A$2:$A$5</f>
             </numRef>
           </cat>
           <val>

</xml_diff>